<commit_message>
add FirstMonthPath and Motivation sheet
</commit_message>
<xml_diff>
--- a/XLSXProject/data/Result.xlsx
+++ b/XLSXProject/data/Result.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="525" windowWidth="18855" windowHeight="11190"/>
+    <workbookView xWindow="150" yWindow="570" windowWidth="18855" windowHeight="10680"/>
   </bookViews>
   <sheets>
-    <sheet name="Result" sheetId="1" r:id="rId1"/>
+    <sheet name="1-15 Операторы" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -507,10 +507,17 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">

</xml_diff>